<commit_message>
update add bot whatsapp
</commit_message>
<xml_diff>
--- a/recipients.xlsx
+++ b/recipients.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="9">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="55" uniqueCount="55">
   <si>
     <t xml:space="preserve">email</t>
   </si>
@@ -31,22 +31,160 @@
     <t xml:space="preserve">group</t>
   </si>
   <si>
-    <t xml:space="preserve">soranatascincinadi@gmail.com</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Sorantas Cincinadi</t>
-  </si>
-  <si>
-    <t xml:space="preserve">angelshroom666@gmail.com</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Anggara</t>
-  </si>
-  <si>
-    <t xml:space="preserve">edikresnha@gmail.com</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Edi Krisna</t>
+    <t xml:space="preserve">afnimahiya@gmail.com</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Nur Afni Mahiya Usemahu</t>
+  </si>
+  <si>
+    <t xml:space="preserve">tantohar384@gmail.com</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Hartanto</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ariobaskoro@live.com</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Ario Baskoro</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ifantirta.official@gmail.com</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Ifan Tirta Adi</t>
+  </si>
+  <si>
+    <t xml:space="preserve">kholidin.atmadinata@ibm.com</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Kholidin Alkhahfi</t>
+  </si>
+  <si>
+    <t xml:space="preserve">arliramdhani@gmail.com</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Arli Ramdhani</t>
+  </si>
+  <si>
+    <t xml:space="preserve">louisa.gcom@gmail.com</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Louisa Veronica Hartono</t>
+  </si>
+  <si>
+    <t xml:space="preserve">m.zamronnii@gmail.com</t>
+  </si>
+  <si>
+    <t xml:space="preserve">M Zamroni</t>
+  </si>
+  <si>
+    <t xml:space="preserve">nawafilhusnul@gmail.com</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Husnul Nawafil</t>
+  </si>
+  <si>
+    <t xml:space="preserve">maysamelda@gmail.com</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Maysa Melda An’umillah</t>
+  </si>
+  <si>
+    <t xml:space="preserve">muhakazm1416@gmail.com</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Muhammad Kamal Azmi</t>
+  </si>
+  <si>
+    <t xml:space="preserve">siraitjonathan22@gmail.com</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Jonathan Benedict Sirait</t>
+  </si>
+  <si>
+    <t xml:space="preserve">kevinforistian@gmail.com</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Kevin Foristian Hondowidjaja</t>
+  </si>
+  <si>
+    <t xml:space="preserve">krinawibisana@gmail.com</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Krina Wibisana</t>
+  </si>
+  <si>
+    <t xml:space="preserve">muhammadlazuardirangkuti@gmail.com</t>
+  </si>
+  <si>
+    <t xml:space="preserve">M Lazuardi </t>
+  </si>
+  <si>
+    <t xml:space="preserve">milzon.ltf@gmail.com</t>
+  </si>
+  <si>
+    <t xml:space="preserve">M Milzon</t>
+  </si>
+  <si>
+    <t xml:space="preserve">petrayohanas@gmail.com</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Petra Yohanna Sitanggang</t>
+  </si>
+  <si>
+    <t xml:space="preserve">nabihbawazir@gmail.com</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Nabih Ibrahim Bawazir</t>
+  </si>
+  <si>
+    <t xml:space="preserve">bayu.kunto1997@gmail.com</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Narendra Bayutama Wibisono</t>
+  </si>
+  <si>
+    <t xml:space="preserve">nikodemusng@gmail.com</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Nikodemus Ng</t>
+  </si>
+  <si>
+    <t xml:space="preserve">nurwidiyanti80@Gmail.com</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Nurwidy</t>
+  </si>
+  <si>
+    <t xml:space="preserve">sulianto.liang@gmail.com</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Sulianto</t>
+  </si>
+  <si>
+    <t xml:space="preserve">hello.rizkiadji@gmail.com</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Rizki Adji Santoso</t>
+  </si>
+  <si>
+    <t xml:space="preserve">rizqiphd@gmail.com</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Rizqi Prima</t>
+  </si>
+  <si>
+    <t xml:space="preserve">vira.avianti@gmail.com</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Vira Avianti</t>
+  </si>
+  <si>
+    <t xml:space="preserve">darshan@asmoro.net</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Darshan Asmoro</t>
   </si>
 </sst>
 </file>
@@ -88,15 +226,15 @@
     <font>
       <sz val="10"/>
       <color rgb="FF0000FF"/>
-      <name val="Times New Roman"/>
-      <family val="1"/>
+      <name val="Arial"/>
+      <family val="2"/>
       <charset val="1"/>
     </font>
     <font>
       <sz val="10"/>
-      <name val="Times New Roman"/>
-      <family val="1"/>
-      <charset val="1"/>
+      <color rgb="FF0000FF"/>
+      <name val="Arial"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="2">
@@ -141,7 +279,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="9">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -159,6 +297,22 @@
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -285,10 +439,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:C7"/>
+  <dimension ref="A1:E29"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C5" activeCellId="0" sqref="C5"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A4" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="G15" activeCellId="0" sqref="G15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" customHeight="true" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -312,52 +466,303 @@
       <c r="A2" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="B2" s="4" t="s">
+      <c r="B2" s="3" t="s">
         <v>4</v>
       </c>
       <c r="C2" s="3" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="B3" s="4" t="s">
+      <c r="B3" s="3" t="s">
         <v>6</v>
       </c>
       <c r="C3" s="3" t="n">
-        <v>3</v>
+        <v>1</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="B4" s="4" t="s">
+      <c r="B4" s="3" t="s">
         <v>8</v>
       </c>
       <c r="C4" s="3" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A5" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="B5" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="C5" s="3" t="n">
+        <v>2</v>
+      </c>
+      <c r="E5" s="5"/>
+    </row>
+    <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A6" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="B6" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="C6" s="3" t="n">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A7" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="B7" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="C7" s="3" t="n">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A8" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="B8" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="C8" s="3" t="n">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A9" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="B9" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="C9" s="6" t="n">
         <v>3</v>
       </c>
     </row>
-    <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A5" s="0"/>
-      <c r="B5" s="0"/>
-    </row>
-    <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A6" s="0"/>
-      <c r="B6" s="0"/>
-    </row>
-    <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A7" s="0"/>
-      <c r="B7" s="0"/>
+    <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A10" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="B10" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="C10" s="3" t="n">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A11" s="7" t="s">
+        <v>21</v>
+      </c>
+      <c r="B11" s="7" t="s">
+        <v>22</v>
+      </c>
+      <c r="C11" s="3" t="n">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A12" s="7" t="s">
+        <v>23</v>
+      </c>
+      <c r="B12" s="7" t="s">
+        <v>24</v>
+      </c>
+      <c r="C12" s="3" t="n">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A13" s="7" t="s">
+        <v>25</v>
+      </c>
+      <c r="B13" s="7" t="s">
+        <v>26</v>
+      </c>
+      <c r="C13" s="3" t="n">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A14" s="7" t="s">
+        <v>27</v>
+      </c>
+      <c r="B14" s="7" t="s">
+        <v>28</v>
+      </c>
+      <c r="C14" s="3" t="n">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A15" s="7" t="s">
+        <v>29</v>
+      </c>
+      <c r="B15" s="7" t="s">
+        <v>30</v>
+      </c>
+      <c r="C15" s="3" t="n">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A16" s="7" t="s">
+        <v>31</v>
+      </c>
+      <c r="B16" s="7" t="s">
+        <v>32</v>
+      </c>
+      <c r="C16" s="3" t="n">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A17" s="7" t="s">
+        <v>33</v>
+      </c>
+      <c r="B17" s="7" t="s">
+        <v>34</v>
+      </c>
+      <c r="C17" s="3" t="n">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A18" s="7" t="s">
+        <v>35</v>
+      </c>
+      <c r="B18" s="7" t="s">
+        <v>36</v>
+      </c>
+      <c r="C18" s="3" t="n">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="19" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A19" s="7" t="s">
+        <v>37</v>
+      </c>
+      <c r="B19" s="7" t="s">
+        <v>38</v>
+      </c>
+      <c r="C19" s="3" t="n">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="20" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A20" s="7" t="s">
+        <v>39</v>
+      </c>
+      <c r="B20" s="7" t="s">
+        <v>40</v>
+      </c>
+      <c r="C20" s="3" t="n">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="21" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A21" s="7" t="s">
+        <v>41</v>
+      </c>
+      <c r="B21" s="7" t="s">
+        <v>42</v>
+      </c>
+      <c r="C21" s="3" t="n">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="22" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A22" s="7" t="s">
+        <v>43</v>
+      </c>
+      <c r="B22" s="7" t="s">
+        <v>44</v>
+      </c>
+      <c r="C22" s="3" t="n">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="23" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A23" s="7" t="s">
+        <v>45</v>
+      </c>
+      <c r="B23" s="7" t="s">
+        <v>46</v>
+      </c>
+      <c r="C23" s="3" t="n">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="24" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A24" s="7" t="s">
+        <v>47</v>
+      </c>
+      <c r="B24" s="7" t="s">
+        <v>48</v>
+      </c>
+      <c r="C24" s="3" t="n">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="25" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A25" s="7" t="s">
+        <v>49</v>
+      </c>
+      <c r="B25" s="7" t="s">
+        <v>50</v>
+      </c>
+      <c r="C25" s="3" t="n">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="26" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A26" s="7" t="s">
+        <v>51</v>
+      </c>
+      <c r="B26" s="7" t="s">
+        <v>52</v>
+      </c>
+      <c r="C26" s="3" t="n">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="27" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A27" s="8" t="s">
+        <v>53</v>
+      </c>
+      <c r="B27" s="8" t="s">
+        <v>54</v>
+      </c>
+      <c r="C27" s="3" t="n">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="28" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A28" s="3"/>
+      <c r="B28" s="3"/>
+      <c r="C28" s="3"/>
+    </row>
+    <row r="29" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A29" s="3"/>
+      <c r="B29" s="3"/>
+      <c r="C29" s="3"/>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="A2" r:id="rId1" display="soranatascincinadi@gmail.com"/>
-    <hyperlink ref="A3" r:id="rId2" display="angelshroom666@gmail.com"/>
-    <hyperlink ref="A4" r:id="rId3" display="edikresnha@gmail.com"/>
+    <hyperlink ref="A6" r:id="rId1" display="kholidin.atmadinata@ibm.com"/>
+    <hyperlink ref="A10" r:id="rId2" display="nawafilhusnul@gmail.com"/>
   </hyperlinks>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>

</xml_diff>